<commit_message>
Use ExcelPackage from source with an update at line 561 / ExcelWorksheet.cs
</commit_message>
<xml_diff>
--- a/ConsoleApplication1/Book1.xlsx
+++ b/ConsoleApplication1/Book1.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="21015" windowHeight="9975"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="21015" windowHeight="9975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -474,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -554,4 +555,16 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>